<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@bfd7fcb22baead4e715b2f897c67b5775a5b0b2b 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-SharedDataModelFile.xlsx
+++ b/StructureDefinition-SharedDataModelFile.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2311" uniqueCount="325">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-30T18:30:14+00:00</t>
+    <t>2024-11-25T15:36:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1024,108 +1024,6 @@
   </si>
   <si>
     <t>The type of data contained in this file. Should be as detailed as possible, e.g., Whole Exome Variant Calls.</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile</t>
-  </si>
-  <si>
-    <t>Provides a reference to another file that is related to this one</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.id</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.meta</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.implicitRules</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.language</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.text</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.contained</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.extension</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.modifierExtension</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.identifier</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.status</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.mode</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.title</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.code</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.subject</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.encounter</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.date</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.source</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.orderedBy</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.note</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.id</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.extension</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.modifierExtension</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.flag</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.deleted</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.date</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.entry.item</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.emptyReason</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.file</t>
-  </si>
-  <si>
-    <t>The file to which this related file is related</t>
-  </si>
-  <si>
-    <t>SharedDataModelFile.relatedFile.type</t>
-  </si>
-  <si>
-    <t>The relationship of the file to the parent file in reference</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1328,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ102"/>
+  <dimension ref="A1:AJ71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1439,8 +1337,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="53.5625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="53.5625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="51.109375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="51.109375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
@@ -8722,3174 +8620,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="B72" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>326</v>
-      </c>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-      <c r="P72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q72" s="2"/>
-      <c r="R72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="B73" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="C73" s="2"/>
-      <c r="D73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E73" s="2"/>
-      <c r="F73" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G73" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J73" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K73" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="O73" s="2"/>
-      <c r="P73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q73" s="2"/>
-      <c r="R73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="N74" s="2"/>
-      <c r="O74" s="2"/>
-      <c r="P74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q74" s="2"/>
-      <c r="R74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E75" s="2"/>
-      <c r="F75" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="O75" s="2"/>
-      <c r="P75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q75" s="2"/>
-      <c r="R75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="B76" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="C76" s="2"/>
-      <c r="D76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G76" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K76" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="O76" s="2"/>
-      <c r="P76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q76" s="2"/>
-      <c r="R76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="B77" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="E77" s="2"/>
-      <c r="F77" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G77" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K77" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="O77" s="2"/>
-      <c r="P77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q77" s="2"/>
-      <c r="R77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="B78" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G78" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K78" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="O78" s="2"/>
-      <c r="P78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q78" s="2"/>
-      <c r="R78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF78" t="s" s="2">
-        <v>131</v>
-      </c>
-      <c r="AG78" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH78" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI78" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ78" t="s" s="2">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="B79" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G79" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K79" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="O79" s="2"/>
-      <c r="P79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q79" s="2"/>
-      <c r="R79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF79" t="s" s="2">
-        <v>139</v>
-      </c>
-      <c r="AG79" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH79" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI79" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ79" t="s" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="B80" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="E80" s="2"/>
-      <c r="F80" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G80" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I80" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="J80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K80" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="O80" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="P80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q80" s="2"/>
-      <c r="R80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF80" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="AG80" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH80" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI80" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ80" t="s" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="B81" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="C81" s="2"/>
-      <c r="D81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E81" s="2"/>
-      <c r="F81" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G81" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K81" t="s" s="2">
-        <v>147</v>
-      </c>
-      <c r="L81" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="N81" s="2"/>
-      <c r="O81" s="2"/>
-      <c r="P81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q81" s="2"/>
-      <c r="R81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF81" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI81" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ81" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="B82" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="C82" s="2"/>
-      <c r="D82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E82" s="2"/>
-      <c r="F82" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G82" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I82" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="J82" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K82" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="L82" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="M82" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="N82" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="O82" s="2"/>
-      <c r="P82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q82" s="2"/>
-      <c r="R82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X82" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="Y82" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Z82" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="AA82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF82" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="AG82" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH82" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI82" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ82" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="B83" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="C83" s="2"/>
-      <c r="D83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E83" s="2"/>
-      <c r="F83" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G83" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I83" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="J83" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K83" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="M83" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="O83" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="P83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q83" s="2"/>
-      <c r="R83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X83" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="Y83" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="Z83" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="AA83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF83" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="AG83" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH83" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI83" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ83" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="B84" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="C84" s="2"/>
-      <c r="D84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E84" s="2"/>
-      <c r="F84" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G84" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J84" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K84" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="L84" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="N84" s="2"/>
-      <c r="O84" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="P84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q84" s="2"/>
-      <c r="R84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T84" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="U84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF84" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="AG84" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH84" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI84" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ84" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="B85" t="s" s="2">
-        <v>339</v>
-      </c>
-      <c r="C85" s="2"/>
-      <c r="D85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E85" s="2"/>
-      <c r="F85" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G85" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J85" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K85" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="L85" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="N85" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="O85" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="P85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q85" s="2"/>
-      <c r="R85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X85" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="Y85" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="Z85" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="AA85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF85" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="AG85" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH85" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI85" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ85" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="B86" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="C86" s="2"/>
-      <c r="D86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E86" s="2"/>
-      <c r="F86" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G86" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J86" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K86" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="L86" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="M86" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="O86" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="P86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q86" s="2"/>
-      <c r="R86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF86" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="AG86" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH86" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI86" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ86" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="B87" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="C87" s="2"/>
-      <c r="D87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E87" s="2"/>
-      <c r="F87" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G87" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K87" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="L87" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="N87" s="2"/>
-      <c r="O87" s="2"/>
-      <c r="P87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q87" s="2"/>
-      <c r="R87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF87" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="AG87" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH87" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI87" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ87" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="B88" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E88" s="2"/>
-      <c r="F88" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J88" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K88" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="L88" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="N88" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="O88" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="P88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q88" s="2"/>
-      <c r="R88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF88" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="AG88" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI88" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ88" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="B89" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="C89" s="2"/>
-      <c r="D89" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="E89" s="2"/>
-      <c r="F89" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G89" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J89" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K89" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="M89" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="N89" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="O89" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="P89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q89" s="2"/>
-      <c r="R89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF89" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="AG89" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH89" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI89" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ89" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="B90" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E90" s="2"/>
-      <c r="F90" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G90" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K90" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="L90" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="M90" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="N90" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="O90" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="P90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q90" s="2"/>
-      <c r="R90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X90" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="Y90" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="Z90" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="AA90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF90" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="AG90" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH90" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI90" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ90" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="B91" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="C91" s="2"/>
-      <c r="D91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E91" s="2"/>
-      <c r="F91" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G91" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K91" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="L91" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M91" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="N91" s="2"/>
-      <c r="O91" s="2"/>
-      <c r="P91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q91" s="2"/>
-      <c r="R91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF91" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AG91" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH91" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI91" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ91" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="B92" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="C92" s="2"/>
-      <c r="D92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E92" s="2"/>
-      <c r="F92" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G92" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K92" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="L92" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M92" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="N92" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="O92" s="2"/>
-      <c r="P92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q92" s="2"/>
-      <c r="R92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE92" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF92" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="AG92" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH92" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI92" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AJ92" t="s" s="2">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="B93" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E93" s="2"/>
-      <c r="F93" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G93" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K93" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="L93" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="M93" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="N93" s="2"/>
-      <c r="O93" s="2"/>
-      <c r="P93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q93" s="2"/>
-      <c r="R93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF93" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AG93" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH93" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI93" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ93" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="B94" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="C94" s="2"/>
-      <c r="D94" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="E94" s="2"/>
-      <c r="F94" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G94" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K94" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="L94" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="M94" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="N94" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="O94" s="2"/>
-      <c r="P94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q94" s="2"/>
-      <c r="R94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF94" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="AG94" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH94" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI94" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ94" t="s" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="B95" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="C95" s="2"/>
-      <c r="D95" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="E95" s="2"/>
-      <c r="F95" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G95" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="H95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I95" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="J95" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="K95" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="L95" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="M95" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="N95" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="O95" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="P95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q95" s="2"/>
-      <c r="R95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF95" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AG95" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH95" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AI95" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ95" t="s" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="B96" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="C96" s="2"/>
-      <c r="D96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E96" s="2"/>
-      <c r="F96" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G96" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K96" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="L96" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M96" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="O96" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="P96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q96" s="2"/>
-      <c r="R96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X96" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="Y96" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="Z96" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="AA96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF96" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="AG96" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH96" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI96" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ96" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="B97" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="C97" s="2"/>
-      <c r="D97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E97" s="2"/>
-      <c r="F97" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G97" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I97" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="J97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K97" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="L97" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="M97" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="N97" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="O97" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="P97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q97" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="R97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE97" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF97" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="AG97" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH97" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI97" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="AJ97" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="B98" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="C98" s="2"/>
-      <c r="D98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E98" s="2"/>
-      <c r="F98" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G98" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K98" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="L98" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M98" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="N98" s="2"/>
-      <c r="O98" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="P98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q98" s="2"/>
-      <c r="R98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF98" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AG98" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH98" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI98" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ98" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="B99" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E99" s="2"/>
-      <c r="F99" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G99" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K99" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="L99" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M99" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="N99" s="2"/>
-      <c r="O99" s="2"/>
-      <c r="P99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q99" s="2"/>
-      <c r="R99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF99" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AG99" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH99" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI99" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ99" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="B100" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="C100" s="2"/>
-      <c r="D100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E100" s="2"/>
-      <c r="F100" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G100" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K100" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="L100" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M100" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N100" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="O100" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="P100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q100" s="2"/>
-      <c r="R100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X100" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="Y100" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="Z100" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="AA100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE100" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF100" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AG100" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH100" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI100" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AJ100" t="s" s="2">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="B101" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="C101" s="2"/>
-      <c r="D101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E101" s="2"/>
-      <c r="F101" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G101" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K101" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="L101" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="M101" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="N101" s="2"/>
-      <c r="O101" s="2"/>
-      <c r="P101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q101" s="2"/>
-      <c r="R101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF101" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="AG101" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH101" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI101" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ101" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="B102" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="C102" s="2"/>
-      <c r="D102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="E102" s="2"/>
-      <c r="F102" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="G102" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="H102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="I102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="J102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="K102" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="L102" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="M102" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="N102" s="2"/>
-      <c r="O102" s="2"/>
-      <c r="P102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q102" s="2"/>
-      <c r="R102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="S102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="T102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="U102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="V102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="W102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="X102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AB102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AC102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AD102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AE102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AF102" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="AG102" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AH102" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AI102" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ102" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig-2@7db7a12b642a2bf3c5a3a3989c5b2c9772c91291 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-SharedDataModelFile.xlsx
+++ b/StructureDefinition-SharedDataModelFile.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-11T13:46:00+00:00</t>
+    <t>2025-08-11T15:03:48+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>78</v>
@@ -1660,7 +1660,7 @@
         <v>77</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>78</v>

</xml_diff>